<commit_message>
- initial version of figuring IVs - Added OCRSpec so that we can incorporate more than just rects to scan OCR fields (including whitelist and blacklist)
</commit_message>
<xml_diff>
--- a/data/pokemon.xlsx
+++ b/data/pokemon.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="-20" windowWidth="30540" windowHeight="24980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="test.csv" sheetId="2" r:id="rId2"/>
+    <sheet name="pokemon.csv" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -22,292 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="178">
   <si>
-    <t>Base Attack</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base Defense</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base Stamina</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Primeape</t>
-  </si>
-  <si>
-    <t>Growlithe</t>
-  </si>
-  <si>
-    <t>Arcanine</t>
-  </si>
-  <si>
-    <t>Poliwag</t>
-  </si>
-  <si>
-    <t>Poliwhirl</t>
-  </si>
-  <si>
-    <t>Poliwrath</t>
-  </si>
-  <si>
-    <t>Abra</t>
-  </si>
-  <si>
-    <t>Kadabra</t>
-  </si>
-  <si>
-    <t>Alakazam</t>
-  </si>
-  <si>
-    <t>Machop</t>
-  </si>
-  <si>
-    <t>Machoke</t>
-  </si>
-  <si>
-    <t>Machamp</t>
-  </si>
-  <si>
-    <t>Bellsprout</t>
-  </si>
-  <si>
-    <t>Weepinbell</t>
-  </si>
-  <si>
-    <t>Victreebel</t>
-  </si>
-  <si>
-    <t>Tentacool</t>
-  </si>
-  <si>
-    <t>Tentacruel</t>
-  </si>
-  <si>
-    <t>Geodude</t>
-  </si>
-  <si>
-    <t>Graveler</t>
-  </si>
-  <si>
-    <t>Golem</t>
-  </si>
-  <si>
-    <t>Ponyta</t>
-  </si>
-  <si>
-    <t>Rapidash</t>
-  </si>
-  <si>
-    <t>Slowpoke</t>
-  </si>
-  <si>
-    <t>Slowbro</t>
-  </si>
-  <si>
-    <t>Magnemite</t>
-  </si>
-  <si>
-    <t>Magneton</t>
-  </si>
-  <si>
-    <t>Farfetch'd</t>
-  </si>
-  <si>
-    <t>Doduo</t>
-  </si>
-  <si>
-    <t>Dodrio</t>
-  </si>
-  <si>
-    <t>Seel</t>
-  </si>
-  <si>
-    <t>Dewgong</t>
-  </si>
-  <si>
-    <t>Grimer</t>
-  </si>
-  <si>
-    <t>Muk</t>
-  </si>
-  <si>
-    <t>Shellder</t>
-  </si>
-  <si>
-    <t>Cloyster</t>
-  </si>
-  <si>
-    <t>Gastly</t>
-  </si>
-  <si>
-    <t>Haunter</t>
-  </si>
-  <si>
-    <t>Gengar</t>
-  </si>
-  <si>
-    <t>Onix</t>
-  </si>
-  <si>
-    <t>Drowzee</t>
-  </si>
-  <si>
-    <t>Hypno</t>
-  </si>
-  <si>
-    <t>Krabby</t>
-  </si>
-  <si>
-    <t>Kingler</t>
-  </si>
-  <si>
-    <t>Voltorb</t>
-  </si>
-  <si>
-    <t>Electrode</t>
-  </si>
-  <si>
-    <t>Exeggcute</t>
-  </si>
-  <si>
-    <t>Exeggutor</t>
-  </si>
-  <si>
-    <t>Cubone</t>
-  </si>
-  <si>
-    <t>Marowak</t>
-  </si>
-  <si>
-    <t>Hitmonlee</t>
-  </si>
-  <si>
-    <t>Hitmonchan</t>
-  </si>
-  <si>
-    <t>Lickitung</t>
-  </si>
-  <si>
-    <t>Koffing</t>
-  </si>
-  <si>
-    <t>Weezing</t>
-  </si>
-  <si>
-    <t>Rhyhorn</t>
-  </si>
-  <si>
-    <t>Rhydon</t>
-  </si>
-  <si>
-    <t>Chansey</t>
-  </si>
-  <si>
-    <t>Tangela</t>
-  </si>
-  <si>
-    <t>Kangaskhan</t>
-  </si>
-  <si>
-    <t>Horsea</t>
-  </si>
-  <si>
-    <t>Seadra</t>
-  </si>
-  <si>
-    <t>Goldeen</t>
-  </si>
-  <si>
-    <t>Seaking</t>
-  </si>
-  <si>
-    <t>Staryu</t>
-  </si>
-  <si>
-    <t>Starmie</t>
-  </si>
-  <si>
-    <t>Mr. Mime</t>
-  </si>
-  <si>
-    <t>Scyther</t>
-  </si>
-  <si>
-    <t>Jynx</t>
-  </si>
-  <si>
-    <t>Electabuzz</t>
-  </si>
-  <si>
-    <t>Magmar</t>
-  </si>
-  <si>
-    <t>Pinsir</t>
-  </si>
-  <si>
-    <t>Tauros</t>
-  </si>
-  <si>
-    <t>Magikarp</t>
-  </si>
-  <si>
-    <t>Gyarados</t>
-  </si>
-  <si>
-    <t>Lapras</t>
-  </si>
-  <si>
-    <t>Ditto</t>
-  </si>
-  <si>
-    <t>Eevee</t>
-  </si>
-  <si>
-    <t>Vaporeon</t>
-  </si>
-  <si>
-    <t>Jolteon</t>
-  </si>
-  <si>
-    <t>Flareon</t>
-  </si>
-  <si>
-    <t>Porygon</t>
-  </si>
-  <si>
-    <t>Omanyte</t>
-  </si>
-  <si>
-    <t>Omastar</t>
-  </si>
-  <si>
-    <t>Kabuto</t>
-  </si>
-  <si>
-    <t>Kabutops</t>
-  </si>
-  <si>
-    <t>Aerodactyl</t>
-  </si>
-  <si>
-    <t>Snorlax</t>
-  </si>
-  <si>
-    <t>Articuno</t>
-  </si>
-  <si>
-    <t>Zapdos</t>
-  </si>
-  <si>
-    <t>Moltres</t>
-  </si>
-  <si>
     <t>Dratini</t>
   </si>
   <si>
@@ -436,6 +150,18 @@
   </si>
   <si>
     <t>Metapod</t>
+  </si>
+  <si>
+    <t>baseAttack</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseDefense</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseStamina</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Butterfree</t>
@@ -594,20 +320,285 @@
   <si>
     <t>Mankey</t>
   </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primeape</t>
+  </si>
+  <si>
+    <t>Growlithe</t>
+  </si>
+  <si>
+    <t>Arcanine</t>
+  </si>
+  <si>
+    <t>Poliwag</t>
+  </si>
+  <si>
+    <t>Poliwhirl</t>
+  </si>
+  <si>
+    <t>Poliwrath</t>
+  </si>
+  <si>
+    <t>Abra</t>
+  </si>
+  <si>
+    <t>Kadabra</t>
+  </si>
+  <si>
+    <t>Alakazam</t>
+  </si>
+  <si>
+    <t>Machop</t>
+  </si>
+  <si>
+    <t>Machoke</t>
+  </si>
+  <si>
+    <t>Machamp</t>
+  </si>
+  <si>
+    <t>Bellsprout</t>
+  </si>
+  <si>
+    <t>Weepinbell</t>
+  </si>
+  <si>
+    <t>Victreebel</t>
+  </si>
+  <si>
+    <t>Tentacool</t>
+  </si>
+  <si>
+    <t>Tentacruel</t>
+  </si>
+  <si>
+    <t>Geodude</t>
+  </si>
+  <si>
+    <t>Graveler</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Ponyta</t>
+  </si>
+  <si>
+    <t>Rapidash</t>
+  </si>
+  <si>
+    <t>Slowpoke</t>
+  </si>
+  <si>
+    <t>Slowbro</t>
+  </si>
+  <si>
+    <t>Magnemite</t>
+  </si>
+  <si>
+    <t>Magneton</t>
+  </si>
+  <si>
+    <t>Farfetch'd</t>
+  </si>
+  <si>
+    <t>Doduo</t>
+  </si>
+  <si>
+    <t>Dodrio</t>
+  </si>
+  <si>
+    <t>Seel</t>
+  </si>
+  <si>
+    <t>Dewgong</t>
+  </si>
+  <si>
+    <t>Grimer</t>
+  </si>
+  <si>
+    <t>Muk</t>
+  </si>
+  <si>
+    <t>Shellder</t>
+  </si>
+  <si>
+    <t>Cloyster</t>
+  </si>
+  <si>
+    <t>Gastly</t>
+  </si>
+  <si>
+    <t>Haunter</t>
+  </si>
+  <si>
+    <t>Gengar</t>
+  </si>
+  <si>
+    <t>Onix</t>
+  </si>
+  <si>
+    <t>Drowzee</t>
+  </si>
+  <si>
+    <t>Hypno</t>
+  </si>
+  <si>
+    <t>Krabby</t>
+  </si>
+  <si>
+    <t>Kingler</t>
+  </si>
+  <si>
+    <t>Voltorb</t>
+  </si>
+  <si>
+    <t>Electrode</t>
+  </si>
+  <si>
+    <t>Exeggcute</t>
+  </si>
+  <si>
+    <t>Exeggutor</t>
+  </si>
+  <si>
+    <t>Cubone</t>
+  </si>
+  <si>
+    <t>Marowak</t>
+  </si>
+  <si>
+    <t>Hitmonlee</t>
+  </si>
+  <si>
+    <t>Hitmonchan</t>
+  </si>
+  <si>
+    <t>Lickitung</t>
+  </si>
+  <si>
+    <t>Koffing</t>
+  </si>
+  <si>
+    <t>Weezing</t>
+  </si>
+  <si>
+    <t>Rhyhorn</t>
+  </si>
+  <si>
+    <t>Rhydon</t>
+  </si>
+  <si>
+    <t>Chansey</t>
+  </si>
+  <si>
+    <t>Tangela</t>
+  </si>
+  <si>
+    <t>Kangaskhan</t>
+  </si>
+  <si>
+    <t>Horsea</t>
+  </si>
+  <si>
+    <t>Seadra</t>
+  </si>
+  <si>
+    <t>Goldeen</t>
+  </si>
+  <si>
+    <t>Seaking</t>
+  </si>
+  <si>
+    <t>Staryu</t>
+  </si>
+  <si>
+    <t>Starmie</t>
+  </si>
+  <si>
+    <t>Mr. Mime</t>
+  </si>
+  <si>
+    <t>Scyther</t>
+  </si>
+  <si>
+    <t>Jynx</t>
+  </si>
+  <si>
+    <t>Electabuzz</t>
+  </si>
+  <si>
+    <t>Magmar</t>
+  </si>
+  <si>
+    <t>Pinsir</t>
+  </si>
+  <si>
+    <t>Tauros</t>
+  </si>
+  <si>
+    <t>Magikarp</t>
+  </si>
+  <si>
+    <t>Gyarados</t>
+  </si>
+  <si>
+    <t>Lapras</t>
+  </si>
+  <si>
+    <t>Ditto</t>
+  </si>
+  <si>
+    <t>Eevee</t>
+  </si>
+  <si>
+    <t>Vaporeon</t>
+  </si>
+  <si>
+    <t>Jolteon</t>
+  </si>
+  <si>
+    <t>Flareon</t>
+  </si>
+  <si>
+    <t>Porygon</t>
+  </si>
+  <si>
+    <t>Omanyte</t>
+  </si>
+  <si>
+    <t>Omastar</t>
+  </si>
+  <si>
+    <t>Kabuto</t>
+  </si>
+  <si>
+    <t>Kabutops</t>
+  </si>
+  <si>
+    <t>Aerodactyl</t>
+  </si>
+  <si>
+    <t>Snorlax</t>
+  </si>
+  <si>
+    <t>Articuno</t>
+  </si>
+  <si>
+    <t>Zapdos</t>
+  </si>
+  <si>
+    <t>Moltres</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -7892,7 +7883,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7934,7 +7925,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7976,7 +7967,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8344,10 +8335,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" thickBot="1">
@@ -8634,58 +8625,58 @@
         <v>0.54263576700000005</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="K33" s="24" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="L33" s="25" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="M33" s="26" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="N33" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="O33" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="P33" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="Q33" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="R33" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="S33" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="T33" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="U33" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="V33" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="20" thickTop="1" thickBot="1">
@@ -8696,7 +8687,7 @@
         <v>0.55079268999999997</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="F34" s="12">
         <v>30</v>
@@ -8766,7 +8757,7 @@
         <v>0.55883057599999997</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>26</v>
       </c>
       <c r="F35" s="12">
         <v>55</v>
@@ -9171,10 +9162,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9185,10 +9174,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K168"/>
+  <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9200,37 +9189,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" thickTop="1">
       <c r="A1" s="29" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16">
@@ -9238,7 +9227,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7">
         <v>45</v>
@@ -9259,12 +9248,12 @@
         <v>45</v>
       </c>
       <c r="I2">
-        <f>2*ROUND((D2+F2)^0.5+H2^0.5,0)</f>
-        <v>34</v>
+        <f>2*ROUND((D2*F2)^0.5+H2^0.5,0)</f>
+        <v>126</v>
       </c>
       <c r="J2">
-        <f>2*ROUND((E2+G2)^0.5+H2^0.5,0)</f>
-        <v>34</v>
+        <f>2*ROUND((E2*G2)^0.5+H2^0.5,0)</f>
+        <v>126</v>
       </c>
       <c r="K2">
         <f>2*C2</f>
@@ -9276,7 +9265,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>123</v>
+        <v>29</v>
       </c>
       <c r="C3" s="7">
         <v>60</v>
@@ -9297,12 +9286,12 @@
         <v>60</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="0">2*ROUND((D3+F3)^0.5+H3^0.5,0)</f>
-        <v>40</v>
+        <f t="shared" ref="I3:I66" si="0">2*ROUND((D3*F3)^0.5+H3^0.5,0)</f>
+        <v>156</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" si="1">2*ROUND((E3+G3)^0.5+H3^0.5,0)</f>
-        <v>40</v>
+        <f t="shared" ref="J3:J66" si="1">2*ROUND((E3*G3)^0.5+H3^0.5,0)</f>
+        <v>158</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K66" si="2">2*C3</f>
@@ -9314,7 +9303,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7">
         <v>80</v>
@@ -9336,11 +9325,11 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>198</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>200</v>
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
@@ -9352,7 +9341,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7">
         <v>39</v>
@@ -9374,11 +9363,11 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
@@ -9390,7 +9379,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>126</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7">
         <v>58</v>
@@ -9412,11 +9401,11 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
@@ -9428,7 +9417,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>127</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7">
         <v>78</v>
@@ -9450,11 +9439,11 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>212</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>182</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
@@ -9466,7 +9455,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="C8" s="7">
         <v>44</v>
@@ -9488,11 +9477,11 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
@@ -9504,7 +9493,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7">
         <v>59</v>
@@ -9526,11 +9515,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
@@ -9542,7 +9531,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7">
         <v>79</v>
@@ -9564,11 +9553,11 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>222</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
@@ -9580,7 +9569,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7">
         <v>45</v>
@@ -9602,11 +9591,11 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
@@ -9618,7 +9607,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7">
         <v>50</v>
@@ -9640,11 +9629,11 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
@@ -9656,7 +9645,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7">
         <v>60</v>
@@ -9678,11 +9667,11 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
@@ -9694,7 +9683,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="C14" s="7">
         <v>40</v>
@@ -9716,11 +9705,11 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
@@ -9732,7 +9721,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="C15" s="7">
         <v>45</v>
@@ -9754,11 +9743,11 @@
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
@@ -9770,7 +9759,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7">
         <v>65</v>
@@ -9792,11 +9781,11 @@
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
@@ -9808,7 +9797,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="C17" s="7">
         <v>40</v>
@@ -9830,11 +9819,11 @@
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
@@ -9846,7 +9835,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>138</v>
+        <v>47</v>
       </c>
       <c r="C18" s="7">
         <v>63</v>
@@ -9868,11 +9857,11 @@
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
@@ -9884,7 +9873,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>139</v>
+        <v>48</v>
       </c>
       <c r="C19" s="7">
         <v>83</v>
@@ -9906,11 +9895,11 @@
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
@@ -9922,7 +9911,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="C20" s="7">
         <v>30</v>
@@ -9944,11 +9933,11 @@
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
@@ -9960,7 +9949,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>141</v>
+        <v>50</v>
       </c>
       <c r="C21" s="7">
         <v>55</v>
@@ -9982,11 +9971,11 @@
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
@@ -9998,7 +9987,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="C22" s="7">
         <v>40</v>
@@ -10020,11 +10009,11 @@
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
@@ -10036,7 +10025,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="C23" s="7">
         <v>65</v>
@@ -10058,11 +10047,11 @@
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="J23">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
@@ -10074,7 +10063,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>144</v>
+        <v>53</v>
       </c>
       <c r="C24" s="7">
         <v>35</v>
@@ -10096,11 +10085,11 @@
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
@@ -10112,7 +10101,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>145</v>
+        <v>54</v>
       </c>
       <c r="C25" s="7">
         <v>60</v>
@@ -10134,11 +10123,11 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="J25">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
@@ -10150,7 +10139,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>146</v>
+        <v>55</v>
       </c>
       <c r="C26" s="7">
         <v>35</v>
@@ -10172,11 +10161,11 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="J26">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
@@ -10188,7 +10177,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="C27" s="7">
         <v>60</v>
@@ -10210,11 +10199,11 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="J27">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
@@ -10226,7 +10215,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="C28" s="7">
         <v>50</v>
@@ -10248,11 +10237,11 @@
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="J28">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="K28">
         <f t="shared" si="2"/>
@@ -10264,7 +10253,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>149</v>
+        <v>58</v>
       </c>
       <c r="C29" s="7">
         <v>75</v>
@@ -10286,11 +10275,11 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="J29">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
@@ -10302,7 +10291,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>150</v>
+        <v>59</v>
       </c>
       <c r="C30" s="7">
         <v>55</v>
@@ -10324,11 +10313,11 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="J30">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
@@ -10340,7 +10329,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
       <c r="C31" s="7">
         <v>70</v>
@@ -10362,11 +10351,11 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="J31">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
@@ -10378,7 +10367,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>152</v>
+        <v>61</v>
       </c>
       <c r="C32" s="7">
         <v>90</v>
@@ -10400,11 +10389,11 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>184</v>
       </c>
       <c r="J32">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="K32">
         <f t="shared" si="2"/>
@@ -10416,7 +10405,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="C33" s="7">
         <v>46</v>
@@ -10438,11 +10427,11 @@
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="J33">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="K33">
         <f t="shared" si="2"/>
@@ -10454,7 +10443,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>154</v>
+        <v>63</v>
       </c>
       <c r="C34" s="7">
         <v>61</v>
@@ -10476,11 +10465,11 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="J34">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="K34">
         <f t="shared" si="2"/>
@@ -10492,7 +10481,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>155</v>
+        <v>64</v>
       </c>
       <c r="C35" s="7">
         <v>81</v>
@@ -10514,11 +10503,11 @@
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="J35">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="K35">
         <f t="shared" si="2"/>
@@ -10530,7 +10519,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>156</v>
+        <v>65</v>
       </c>
       <c r="C36" s="7">
         <v>70</v>
@@ -10552,11 +10541,11 @@
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="J36">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="K36">
         <f t="shared" si="2"/>
@@ -10568,7 +10557,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>157</v>
+        <v>66</v>
       </c>
       <c r="C37" s="7">
         <v>95</v>
@@ -10590,11 +10579,11 @@
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="J37">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="K37">
         <f t="shared" si="2"/>
@@ -10606,7 +10595,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="C38" s="7">
         <v>38</v>
@@ -10628,11 +10617,11 @@
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="J38">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="K38">
         <f t="shared" si="2"/>
@@ -10644,7 +10633,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>159</v>
+        <v>68</v>
       </c>
       <c r="C39" s="7">
         <v>73</v>
@@ -10666,11 +10655,11 @@
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="J39">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>194</v>
       </c>
       <c r="K39">
         <f t="shared" si="2"/>
@@ -10682,7 +10671,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>160</v>
+        <v>69</v>
       </c>
       <c r="C40" s="7">
         <v>115</v>
@@ -10704,11 +10693,11 @@
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="J40">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="K40">
         <f t="shared" si="2"/>
@@ -10720,7 +10709,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>161</v>
+        <v>70</v>
       </c>
       <c r="C41" s="7">
         <v>140</v>
@@ -10742,11 +10731,11 @@
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>168</v>
       </c>
       <c r="J41">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="K41">
         <f t="shared" si="2"/>
@@ -10758,7 +10747,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="C42" s="7">
         <v>40</v>
@@ -10780,11 +10769,11 @@
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="J42">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="K42">
         <f t="shared" si="2"/>
@@ -10796,7 +10785,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="C43" s="7">
         <v>75</v>
@@ -10818,11 +10807,11 @@
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>164</v>
       </c>
       <c r="J43">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>164</v>
       </c>
       <c r="K43">
         <f t="shared" si="2"/>
@@ -10834,7 +10823,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
       <c r="C44" s="7">
         <v>45</v>
@@ -10856,11 +10845,11 @@
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>134</v>
       </c>
       <c r="J44">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="K44">
         <f t="shared" si="2"/>
@@ -10872,7 +10861,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="C45" s="7">
         <v>60</v>
@@ -10894,11 +10883,11 @@
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="J45">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>158</v>
       </c>
       <c r="K45">
         <f t="shared" si="2"/>
@@ -10910,7 +10899,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>166</v>
+        <v>75</v>
       </c>
       <c r="C46" s="7">
         <v>75</v>
@@ -10932,11 +10921,11 @@
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="J46">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="K46">
         <f t="shared" si="2"/>
@@ -10948,7 +10937,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>167</v>
+        <v>76</v>
       </c>
       <c r="C47" s="7">
         <v>35</v>
@@ -10970,11 +10959,11 @@
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="J47">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="K47">
         <f t="shared" si="2"/>
@@ -10986,7 +10975,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>168</v>
+        <v>77</v>
       </c>
       <c r="C48" s="7">
         <v>60</v>
@@ -11008,11 +10997,11 @@
       </c>
       <c r="I48">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="J48">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="K48">
         <f t="shared" si="2"/>
@@ -11024,7 +11013,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="C49" s="7">
         <v>60</v>
@@ -11046,11 +11035,11 @@
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="J49">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="K49">
         <f t="shared" si="2"/>
@@ -11062,7 +11051,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="C50" s="7">
         <v>70</v>
@@ -11084,11 +11073,11 @@
       </c>
       <c r="I50">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>172</v>
       </c>
       <c r="J50">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="K50">
         <f t="shared" si="2"/>
@@ -11100,7 +11089,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="C51" s="7">
         <v>10</v>
@@ -11122,11 +11111,11 @@
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="J51">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K51">
         <f t="shared" si="2"/>
@@ -11138,7 +11127,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>172</v>
+        <v>81</v>
       </c>
       <c r="C52" s="7">
         <v>35</v>
@@ -11160,11 +11149,11 @@
       </c>
       <c r="I52">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="J52">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="K52">
         <f t="shared" si="2"/>
@@ -11176,7 +11165,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>173</v>
+        <v>82</v>
       </c>
       <c r="C53" s="7">
         <v>40</v>
@@ -11198,11 +11187,11 @@
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="J53">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="K53">
         <f t="shared" si="2"/>
@@ -11214,7 +11203,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>174</v>
+        <v>83</v>
       </c>
       <c r="C54" s="7">
         <v>65</v>
@@ -11236,11 +11225,11 @@
       </c>
       <c r="I54">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="J54">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="K54">
         <f t="shared" si="2"/>
@@ -11252,7 +11241,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>175</v>
+        <v>84</v>
       </c>
       <c r="C55" s="7">
         <v>50</v>
@@ -11274,11 +11263,11 @@
       </c>
       <c r="I55">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="J55">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="K55">
         <f t="shared" si="2"/>
@@ -11290,7 +11279,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>176</v>
+        <v>85</v>
       </c>
       <c r="C56" s="7">
         <v>80</v>
@@ -11312,11 +11301,11 @@
       </c>
       <c r="I56">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>194</v>
       </c>
       <c r="J56">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="K56">
         <f t="shared" si="2"/>
@@ -11328,7 +11317,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>177</v>
+        <v>86</v>
       </c>
       <c r="C57" s="7">
         <v>40</v>
@@ -11350,11 +11339,11 @@
       </c>
       <c r="I57">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="J57">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="K57">
         <f t="shared" si="2"/>
@@ -11366,7 +11355,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C58" s="7">
         <v>65</v>
@@ -11388,11 +11377,11 @@
       </c>
       <c r="I58">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="J58">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="K58">
         <f t="shared" si="2"/>
@@ -11404,7 +11393,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C59" s="7">
         <v>55</v>
@@ -11426,11 +11415,11 @@
       </c>
       <c r="I59">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="J59">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="K59">
         <f t="shared" si="2"/>
@@ -11442,7 +11431,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="C60" s="7">
         <v>90</v>
@@ -11464,11 +11453,11 @@
       </c>
       <c r="I60">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>230</v>
       </c>
       <c r="J60">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="K60">
         <f t="shared" si="2"/>
@@ -11480,7 +11469,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C61" s="7">
         <v>40</v>
@@ -11502,11 +11491,11 @@
       </c>
       <c r="I61">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="J61">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="K61">
         <f t="shared" si="2"/>
@@ -11518,7 +11507,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="C62" s="7">
         <v>65</v>
@@ -11540,11 +11529,11 @@
       </c>
       <c r="I62">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="J62">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="K62">
         <f t="shared" si="2"/>
@@ -11556,7 +11545,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="C63" s="7">
         <v>90</v>
@@ -11578,11 +11567,11 @@
       </c>
       <c r="I63">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="J63">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="K63">
         <f t="shared" si="2"/>
@@ -11594,7 +11583,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="C64" s="7">
         <v>25</v>
@@ -11616,11 +11605,11 @@
       </c>
       <c r="I64">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="J64">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="K64">
         <f t="shared" si="2"/>
@@ -11632,7 +11621,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="C65" s="7">
         <v>40</v>
@@ -11654,11 +11643,11 @@
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="J65">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="K65">
         <f t="shared" si="2"/>
@@ -11670,7 +11659,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="C66" s="7">
         <v>55</v>
@@ -11692,11 +11681,11 @@
       </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="J66">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="K66">
         <f t="shared" si="2"/>
@@ -11708,7 +11697,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C67" s="7">
         <v>70</v>
@@ -11729,12 +11718,12 @@
         <v>35</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I130" si="3">2*ROUND((D67+F67)^0.5+H67^0.5,0)</f>
-        <v>34</v>
+        <f t="shared" ref="I67:I130" si="3">2*ROUND((D67*F67)^0.5+H67^0.5,0)</f>
+        <v>118</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J130" si="4">2*ROUND((E67+G67)^0.5+H67^0.5,0)</f>
-        <v>30</v>
+        <f t="shared" ref="J67:J130" si="4">2*ROUND((E67*G67)^0.5+H67^0.5,0)</f>
+        <v>96</v>
       </c>
       <c r="K67">
         <f t="shared" ref="K67:K130" si="5">2*C67</f>
@@ -11746,7 +11735,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="C68" s="7">
         <v>80</v>
@@ -11768,11 +11757,11 @@
       </c>
       <c r="I68">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="J68">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="K68">
         <f t="shared" si="5"/>
@@ -11784,7 +11773,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="C69" s="7">
         <v>90</v>
@@ -11806,11 +11795,11 @@
       </c>
       <c r="I69">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>198</v>
       </c>
       <c r="J69">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>180</v>
       </c>
       <c r="K69">
         <f t="shared" si="5"/>
@@ -11822,7 +11811,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="C70" s="7">
         <v>50</v>
@@ -11844,11 +11833,11 @@
       </c>
       <c r="I70">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>158</v>
       </c>
       <c r="J70">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="K70">
         <f t="shared" si="5"/>
@@ -11860,7 +11849,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C71" s="7">
         <v>65</v>
@@ -11882,11 +11871,11 @@
       </c>
       <c r="I71">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="J71">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="K71">
         <f t="shared" si="5"/>
@@ -11898,7 +11887,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="C72" s="7">
         <v>80</v>
@@ -11920,11 +11909,11 @@
       </c>
       <c r="I72">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>222</v>
       </c>
       <c r="J72">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="K72">
         <f t="shared" si="5"/>
@@ -11936,7 +11925,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C73" s="7">
         <v>40</v>
@@ -11958,11 +11947,11 @@
       </c>
       <c r="I73">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="J73">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="K73">
         <f t="shared" si="5"/>
@@ -11974,7 +11963,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="C74" s="7">
         <v>80</v>
@@ -11996,11 +11985,11 @@
       </c>
       <c r="I74">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="J74">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="K74">
         <f t="shared" si="5"/>
@@ -12012,7 +12001,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="C75" s="7">
         <v>40</v>
@@ -12034,11 +12023,11 @@
       </c>
       <c r="I75">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="J75">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="K75">
         <f t="shared" si="5"/>
@@ -12050,7 +12039,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="C76" s="7">
         <v>55</v>
@@ -12072,11 +12061,11 @@
       </c>
       <c r="I76">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="J76">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="K76">
         <f t="shared" si="5"/>
@@ -12088,7 +12077,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="C77" s="7">
         <v>80</v>
@@ -12110,11 +12099,11 @@
       </c>
       <c r="I77">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="J77">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>198</v>
       </c>
       <c r="K77">
         <f t="shared" si="5"/>
@@ -12126,7 +12115,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C78" s="7">
         <v>50</v>
@@ -12148,11 +12137,11 @@
       </c>
       <c r="I78">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="J78">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="K78">
         <f t="shared" si="5"/>
@@ -12164,7 +12153,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="C79" s="7">
         <v>65</v>
@@ -12186,11 +12175,11 @@
       </c>
       <c r="I79">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="J79">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="K79">
         <f t="shared" si="5"/>
@@ -12202,7 +12191,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="C80" s="7">
         <v>90</v>
@@ -12224,11 +12213,11 @@
       </c>
       <c r="I80">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="J80">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="K80">
         <f t="shared" si="5"/>
@@ -12240,7 +12229,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="28" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="C81" s="7">
         <v>95</v>
@@ -12262,11 +12251,11 @@
       </c>
       <c r="I81">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="J81">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="K81">
         <f t="shared" si="5"/>
@@ -12278,7 +12267,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="C82" s="7">
         <v>25</v>
@@ -12300,11 +12289,11 @@
       </c>
       <c r="I82">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="J82">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="K82">
         <f t="shared" si="5"/>
@@ -12316,7 +12305,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="28" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C83" s="7">
         <v>50</v>
@@ -12338,11 +12327,11 @@
       </c>
       <c r="I83">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="J83">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="K83">
         <f t="shared" si="5"/>
@@ -12354,7 +12343,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="C84" s="7">
         <v>52</v>
@@ -12376,11 +12365,11 @@
       </c>
       <c r="I84">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="J84">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="K84">
         <f t="shared" si="5"/>
@@ -12392,7 +12381,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="C85" s="7">
         <v>35</v>
@@ -12414,11 +12403,11 @@
       </c>
       <c r="I85">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="J85">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="K85">
         <f t="shared" si="5"/>
@@ -12430,7 +12419,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="C86" s="7">
         <v>60</v>
@@ -12452,11 +12441,11 @@
       </c>
       <c r="I86">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>182</v>
       </c>
       <c r="J86">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="K86">
         <f t="shared" si="5"/>
@@ -12468,7 +12457,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="C87" s="7">
         <v>65</v>
@@ -12490,11 +12479,11 @@
       </c>
       <c r="I87">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="J87">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="K87">
         <f t="shared" si="5"/>
@@ -12506,7 +12495,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="C88" s="7">
         <v>90</v>
@@ -12528,11 +12517,11 @@
       </c>
       <c r="I88">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="J88">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="K88">
         <f t="shared" si="5"/>
@@ -12544,7 +12533,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="C89" s="7">
         <v>80</v>
@@ -12566,11 +12555,11 @@
       </c>
       <c r="I89">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="J89">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="K89">
         <f t="shared" si="5"/>
@@ -12582,7 +12571,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="C90" s="7">
         <v>105</v>
@@ -12604,11 +12593,11 @@
       </c>
       <c r="I90">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>180</v>
       </c>
       <c r="J90">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>188</v>
       </c>
       <c r="K90">
         <f t="shared" si="5"/>
@@ -12620,7 +12609,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="C91" s="7">
         <v>30</v>
@@ -12642,11 +12631,11 @@
       </c>
       <c r="I91">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="J91">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="K91">
         <f t="shared" si="5"/>
@@ -12658,7 +12647,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="C92" s="7">
         <v>50</v>
@@ -12680,11 +12669,11 @@
       </c>
       <c r="I92">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="J92">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="K92">
         <f t="shared" si="5"/>
@@ -12696,7 +12685,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="C93" s="7">
         <v>30</v>
@@ -12718,11 +12707,11 @@
       </c>
       <c r="I93">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="J93">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="K93">
         <f t="shared" si="5"/>
@@ -12734,7 +12723,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C94" s="7">
         <v>45</v>
@@ -12756,11 +12745,11 @@
       </c>
       <c r="I94">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="J94">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="K94">
         <f t="shared" si="5"/>
@@ -12772,7 +12761,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="C95" s="7">
         <v>60</v>
@@ -12794,11 +12783,11 @@
       </c>
       <c r="I95">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="J95">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="K95">
         <f t="shared" si="5"/>
@@ -12810,7 +12799,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="C96" s="7">
         <v>35</v>
@@ -12832,11 +12821,11 @@
       </c>
       <c r="I96">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="J96">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>186</v>
       </c>
       <c r="K96">
         <f t="shared" si="5"/>
@@ -12848,7 +12837,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="C97" s="7">
         <v>60</v>
@@ -12870,11 +12859,11 @@
       </c>
       <c r="I97">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="J97">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="K97">
         <f t="shared" si="5"/>
@@ -12886,7 +12875,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C98" s="7">
         <v>85</v>
@@ -12908,11 +12897,11 @@
       </c>
       <c r="I98">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="J98">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="K98">
         <f t="shared" si="5"/>
@@ -12924,7 +12913,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C99" s="7">
         <v>30</v>
@@ -12946,11 +12935,11 @@
       </c>
       <c r="I99">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="J99">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="K99">
         <f t="shared" si="5"/>
@@ -12962,7 +12951,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="C100" s="7">
         <v>55</v>
@@ -12984,11 +12973,11 @@
       </c>
       <c r="I100">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="J100">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="K100">
         <f t="shared" si="5"/>
@@ -13000,7 +12989,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="C101" s="7">
         <v>40</v>
@@ -13022,11 +13011,11 @@
       </c>
       <c r="I101">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="J101">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="K101">
         <f t="shared" si="5"/>
@@ -13038,7 +13027,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="C102" s="7">
         <v>60</v>
@@ -13060,11 +13049,11 @@
       </c>
       <c r="I102">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="J102">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K102">
         <f t="shared" si="5"/>
@@ -13076,7 +13065,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="C103" s="7">
         <v>60</v>
@@ -13098,11 +13087,11 @@
       </c>
       <c r="I103">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="J103">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="K103">
         <f t="shared" si="5"/>
@@ -13114,7 +13103,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="C104" s="7">
         <v>95</v>
@@ -13136,11 +13125,11 @@
       </c>
       <c r="I104">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="J104">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="K104">
         <f t="shared" si="5"/>
@@ -13152,7 +13141,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="C105" s="7">
         <v>50</v>
@@ -13174,11 +13163,11 @@
       </c>
       <c r="I105">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="J105">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="K105">
         <f t="shared" si="5"/>
@@ -13190,7 +13179,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="C106" s="7">
         <v>60</v>
@@ -13212,11 +13201,11 @@
       </c>
       <c r="I106">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="J106">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="K106">
         <f t="shared" si="5"/>
@@ -13228,7 +13217,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="C107" s="7">
         <v>50</v>
@@ -13250,11 +13239,11 @@
       </c>
       <c r="I107">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="J107">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>172</v>
       </c>
       <c r="K107">
         <f t="shared" si="5"/>
@@ -13266,7 +13255,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="C108" s="7">
         <v>50</v>
@@ -13288,11 +13277,11 @@
       </c>
       <c r="I108">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>138</v>
       </c>
       <c r="J108">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="K108">
         <f t="shared" si="5"/>
@@ -13304,7 +13293,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="C109" s="7">
         <v>90</v>
@@ -13326,11 +13315,11 @@
       </c>
       <c r="I109">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="J109">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="K109">
         <f t="shared" si="5"/>
@@ -13342,7 +13331,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C110" s="7">
         <v>40</v>
@@ -13364,11 +13353,11 @@
       </c>
       <c r="I110">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="J110">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="K110">
         <f t="shared" si="5"/>
@@ -13380,7 +13369,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="C111" s="7">
         <v>65</v>
@@ -13402,11 +13391,11 @@
       </c>
       <c r="I111">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="J111">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>198</v>
       </c>
       <c r="K111">
         <f t="shared" si="5"/>
@@ -13418,7 +13407,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="C112" s="7">
         <v>80</v>
@@ -13440,11 +13429,11 @@
       </c>
       <c r="I112">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="J112">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="K112">
         <f t="shared" si="5"/>
@@ -13456,7 +13445,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>59</v>
+        <v>143</v>
       </c>
       <c r="C113" s="7">
         <v>105</v>
@@ -13478,11 +13467,11 @@
       </c>
       <c r="I113">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>166</v>
       </c>
       <c r="J113">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="K113">
         <f t="shared" si="5"/>
@@ -13494,7 +13483,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>60</v>
+        <v>144</v>
       </c>
       <c r="C114" s="7">
         <v>250</v>
@@ -13516,11 +13505,11 @@
       </c>
       <c r="I114">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="J114">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="K114">
         <f t="shared" si="5"/>
@@ -13532,7 +13521,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="C115" s="7">
         <v>65</v>
@@ -13554,11 +13543,11 @@
       </c>
       <c r="I115">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="J115">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="K115">
         <f t="shared" si="5"/>
@@ -13570,7 +13559,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="C116" s="7">
         <v>105</v>
@@ -13592,11 +13581,11 @@
       </c>
       <c r="I116">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="J116">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="K116">
         <f t="shared" si="5"/>
@@ -13608,7 +13597,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="28" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="C117" s="7">
         <v>30</v>
@@ -13630,11 +13619,11 @@
       </c>
       <c r="I117">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="J117">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="K117">
         <f t="shared" si="5"/>
@@ -13646,7 +13635,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="28" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="C118" s="7">
         <v>55</v>
@@ -13668,11 +13657,11 @@
       </c>
       <c r="I118">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="J118">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="K118">
         <f t="shared" si="5"/>
@@ -13684,7 +13673,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="28" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="C119" s="7">
         <v>45</v>
@@ -13706,11 +13695,11 @@
       </c>
       <c r="I119">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="J119">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="K119">
         <f t="shared" si="5"/>
@@ -13722,7 +13711,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="C120" s="7">
         <v>80</v>
@@ -13744,11 +13733,11 @@
       </c>
       <c r="I120">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="J120">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="K120">
         <f t="shared" si="5"/>
@@ -13760,7 +13749,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="C121" s="7">
         <v>30</v>
@@ -13782,11 +13771,11 @@
       </c>
       <c r="I121">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="J121">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="K121">
         <f t="shared" si="5"/>
@@ -13798,7 +13787,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="C122" s="7">
         <v>60</v>
@@ -13820,11 +13809,11 @@
       </c>
       <c r="I122">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>194</v>
       </c>
       <c r="J122">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="K122">
         <f t="shared" si="5"/>
@@ -13836,7 +13825,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="C123" s="7">
         <v>40</v>
@@ -13858,11 +13847,11 @@
       </c>
       <c r="I123">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="J123">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="K123">
         <f t="shared" si="5"/>
@@ -13874,7 +13863,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="C124" s="7">
         <v>70</v>
@@ -13896,11 +13885,11 @@
       </c>
       <c r="I124">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="J124">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>180</v>
       </c>
       <c r="K124">
         <f t="shared" si="5"/>
@@ -13912,7 +13901,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="C125" s="7">
         <v>65</v>
@@ -13934,11 +13923,11 @@
       </c>
       <c r="I125">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="J125">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="K125">
         <f t="shared" si="5"/>
@@ -13950,7 +13939,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
       <c r="C126" s="7">
         <v>65</v>
@@ -13972,11 +13961,11 @@
       </c>
       <c r="I126">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="J126">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="K126">
         <f t="shared" si="5"/>
@@ -13988,7 +13977,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="C127" s="7">
         <v>65</v>
@@ -14010,11 +13999,11 @@
       </c>
       <c r="I127">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>214</v>
       </c>
       <c r="J127">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="K127">
         <f t="shared" si="5"/>
@@ -14026,7 +14015,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="28" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="C128" s="7">
         <v>65</v>
@@ -14048,11 +14037,11 @@
       </c>
       <c r="I128">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>184</v>
       </c>
       <c r="J128">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="K128">
         <f t="shared" si="5"/>
@@ -14064,7 +14053,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="28" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="C129" s="7">
         <v>75</v>
@@ -14086,11 +14075,11 @@
       </c>
       <c r="I129">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="J129">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>184</v>
       </c>
       <c r="K129">
         <f t="shared" si="5"/>
@@ -14102,7 +14091,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="C130" s="7">
         <v>20</v>
@@ -14124,11 +14113,11 @@
       </c>
       <c r="I130">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J130">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="K130">
         <f t="shared" si="5"/>
@@ -14140,7 +14129,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>77</v>
+        <v>161</v>
       </c>
       <c r="C131" s="7">
         <v>95</v>
@@ -14161,12 +14150,12 @@
         <v>81</v>
       </c>
       <c r="I131">
-        <f t="shared" ref="I131:I152" si="6">2*ROUND((D131+F131)^0.5+H131^0.5,0)</f>
-        <v>46</v>
+        <f t="shared" ref="I131:I152" si="6">2*ROUND((D131*F131)^0.5+H131^0.5,0)</f>
+        <v>192</v>
       </c>
       <c r="J131">
-        <f t="shared" ref="J131:J152" si="7">2*ROUND((E131+G131)^0.5+H131^0.5,0)</f>
-        <v>44</v>
+        <f t="shared" ref="J131:J152" si="7">2*ROUND((E131*G131)^0.5+H131^0.5,0)</f>
+        <v>196</v>
       </c>
       <c r="K131">
         <f t="shared" ref="K131:K152" si="8">2*C131</f>
@@ -14178,7 +14167,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="28" t="s">
-        <v>78</v>
+        <v>162</v>
       </c>
       <c r="C132" s="7">
         <v>130</v>
@@ -14200,11 +14189,11 @@
       </c>
       <c r="I132">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="J132">
         <f t="shared" si="7"/>
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="K132">
         <f t="shared" si="8"/>
@@ -14216,7 +14205,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="28" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="C133" s="7">
         <v>48</v>
@@ -14238,11 +14227,11 @@
       </c>
       <c r="I133">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="J133">
         <f t="shared" si="7"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="K133">
         <f t="shared" si="8"/>
@@ -14254,7 +14243,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="28" t="s">
-        <v>80</v>
+        <v>164</v>
       </c>
       <c r="C134" s="7">
         <v>55</v>
@@ -14276,11 +14265,11 @@
       </c>
       <c r="I134">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="J134">
         <f t="shared" si="7"/>
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="K134">
         <f t="shared" si="8"/>
@@ -14292,7 +14281,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="28" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="C135" s="7">
         <v>130</v>
@@ -14314,11 +14303,11 @@
       </c>
       <c r="I135">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="J135">
         <f t="shared" si="7"/>
-        <v>42</v>
+        <v>168</v>
       </c>
       <c r="K135">
         <f t="shared" si="8"/>
@@ -14330,7 +14319,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="28" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="C136" s="7">
         <v>65</v>
@@ -14352,11 +14341,11 @@
       </c>
       <c r="I136">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="J136">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K136">
         <f t="shared" si="8"/>
@@ -14368,7 +14357,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="28" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="C137" s="7">
         <v>65</v>
@@ -14390,11 +14379,11 @@
       </c>
       <c r="I137">
         <f t="shared" si="6"/>
-        <v>46</v>
+        <v>238</v>
       </c>
       <c r="J137">
         <f t="shared" si="7"/>
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="K137">
         <f t="shared" si="8"/>
@@ -14406,7 +14395,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="28" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="C138" s="7">
         <v>65</v>
@@ -14428,11 +14417,11 @@
       </c>
       <c r="I138">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>156</v>
       </c>
       <c r="J138">
         <f t="shared" si="7"/>
-        <v>36</v>
+        <v>158</v>
       </c>
       <c r="K138">
         <f t="shared" si="8"/>
@@ -14444,7 +14433,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="28" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="C139" s="7">
         <v>35</v>
@@ -14466,11 +14455,11 @@
       </c>
       <c r="I139">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="J139">
         <f t="shared" si="7"/>
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="K139">
         <f t="shared" si="8"/>
@@ -14482,7 +14471,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="28" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="C140" s="7">
         <v>70</v>
@@ -14504,11 +14493,11 @@
       </c>
       <c r="I140">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="J140">
         <f t="shared" si="7"/>
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="K140">
         <f t="shared" si="8"/>
@@ -14520,7 +14509,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="28" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C141" s="7">
         <v>30</v>
@@ -14542,11 +14531,11 @@
       </c>
       <c r="I141">
         <f t="shared" si="6"/>
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="J141">
         <f t="shared" si="7"/>
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="K141">
         <f t="shared" si="8"/>
@@ -14558,7 +14547,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="28" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="C142" s="7">
         <v>60</v>
@@ -14580,11 +14569,11 @@
       </c>
       <c r="I142">
         <f t="shared" si="6"/>
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="J142">
         <f t="shared" si="7"/>
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="K142">
         <f t="shared" si="8"/>
@@ -14596,7 +14585,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="28" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
       <c r="C143" s="7">
         <v>80</v>
@@ -14618,11 +14607,11 @@
       </c>
       <c r="I143">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="J143">
         <f t="shared" si="7"/>
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="K143">
         <f t="shared" si="8"/>
@@ -14634,7 +14623,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="28" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="C144" s="7">
         <v>160</v>
@@ -14656,11 +14645,11 @@
       </c>
       <c r="I144">
         <f t="shared" si="6"/>
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="J144">
         <f t="shared" si="7"/>
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="K144">
         <f t="shared" si="8"/>
@@ -14672,7 +14661,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="28" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
       <c r="C145" s="7">
         <v>90</v>
@@ -14694,11 +14683,11 @@
       </c>
       <c r="I145">
         <f t="shared" si="6"/>
-        <v>46</v>
+        <v>198</v>
       </c>
       <c r="J145">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>242</v>
       </c>
       <c r="K145">
         <f t="shared" si="8"/>
@@ -14710,7 +14699,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="28" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="C146" s="7">
         <v>90</v>
@@ -14732,11 +14721,11 @@
       </c>
       <c r="I146">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>232</v>
       </c>
       <c r="J146">
         <f t="shared" si="7"/>
-        <v>46</v>
+        <v>194</v>
       </c>
       <c r="K146">
         <f t="shared" si="8"/>
@@ -14748,7 +14737,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="28" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
       <c r="C147" s="7">
         <v>90</v>
@@ -14770,11 +14759,11 @@
       </c>
       <c r="I147">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>242</v>
       </c>
       <c r="J147">
         <f t="shared" si="7"/>
-        <v>46</v>
+        <v>194</v>
       </c>
       <c r="K147">
         <f t="shared" si="8"/>
@@ -14786,7 +14775,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="28" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="C148" s="7">
         <v>41</v>
@@ -14808,11 +14797,11 @@
       </c>
       <c r="I148">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="J148">
         <f t="shared" si="7"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="K148">
         <f t="shared" si="8"/>
@@ -14824,7 +14813,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="28" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="C149" s="7">
         <v>61</v>
@@ -14846,11 +14835,11 @@
       </c>
       <c r="I149">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="J149">
         <f t="shared" si="7"/>
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="K149">
         <f t="shared" si="8"/>
@@ -14862,7 +14851,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="28" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="C150" s="7">
         <v>91</v>
@@ -14884,11 +14873,11 @@
       </c>
       <c r="I150">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>250</v>
       </c>
       <c r="J150">
         <f t="shared" si="7"/>
-        <v>46</v>
+        <v>212</v>
       </c>
       <c r="K150">
         <f t="shared" si="8"/>
@@ -14900,7 +14889,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="28" t="s">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="C151" s="7">
         <v>106</v>
@@ -14922,11 +14911,11 @@
       </c>
       <c r="I151">
         <f t="shared" si="6"/>
-        <v>56</v>
+        <v>284</v>
       </c>
       <c r="J151">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>202</v>
       </c>
       <c r="K151">
         <f t="shared" si="8"/>
@@ -14938,7 +14927,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="39" t="s">
-        <v>98</v>
+        <v>4</v>
       </c>
       <c r="C152" s="40">
         <v>100</v>
@@ -14960,29 +14949,19 @@
       </c>
       <c r="I152">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>220</v>
       </c>
       <c r="J152">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>220</v>
       </c>
       <c r="K152">
         <f t="shared" si="8"/>
         <v>200</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="16"/>
-    <row r="157" spans="1:11" ht="16"/>
-    <row r="158" spans="1:11" ht="16"/>
-    <row r="159" spans="1:11" ht="16"/>
-    <row r="160" spans="1:11" ht="16"/>
-    <row r="162" ht="16"/>
-    <row r="165" ht="16"/>
-    <row r="166" ht="16"/>
-    <row r="167" ht="16"/>
-    <row r="168" ht="16"/>
+    <row r="153" spans="1:11" ht="14" thickTop="1"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="National Pokédex"/>

</xml_diff>